<commit_message>
update product backlog according to sprint#1 backlog
</commit_message>
<xml_diff>
--- a/process/ProductBacklog.xlsx
+++ b/process/ProductBacklog.xlsx
@@ -144,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -191,6 +191,19 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="11"/>
       </left>
       <right style="thin">
@@ -209,6 +222,17 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
         <color indexed="13"/>
       </right>
       <top style="thin">
@@ -516,6 +540,19 @@
       </top>
       <bottom style="thin">
         <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,7 +562,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -541,94 +578,103 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1717,7 +1763,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1725,8 +1771,8 @@
   <cols>
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="61.3516" style="1" customWidth="1"/>
-    <col min="3" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1736,260 +1782,282 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" ht="32.25" customHeight="1">
-      <c r="A2" t="s" s="5">
+      <c r="A2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="7">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="7">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" t="s" s="7">
         <v>4</v>
       </c>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" ht="32.2" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10">
+      <c r="C3" s="11"/>
+      <c r="D3" s="12">
         <v>5</v>
       </c>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" ht="32" customHeight="1">
-      <c r="A4" s="11">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="12">
+      <c r="B4" t="s" s="14">
         <v>6</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14">
+      <c r="C4" s="15"/>
+      <c r="D4" s="16">
         <v>6</v>
       </c>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" s="15">
+      <c r="A5" s="17">
         <v>3</v>
       </c>
-      <c r="B5" t="s" s="16">
+      <c r="B5" t="s" s="18">
         <v>7</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18">
+      <c r="C5" s="19"/>
+      <c r="D5" s="20">
         <v>10</v>
       </c>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" s="15">
+      <c r="A6" s="17">
         <v>4</v>
       </c>
-      <c r="B6" t="s" s="16">
+      <c r="B6" t="s" s="18">
         <v>8</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18">
+      <c r="C6" s="19"/>
+      <c r="D6" s="20">
         <v>5</v>
       </c>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="20" customHeight="1">
-      <c r="A7" s="19">
+      <c r="A7" s="21">
         <v>5</v>
       </c>
-      <c r="B7" t="s" s="20">
+      <c r="B7" t="s" s="22">
         <v>9</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22">
+      <c r="C7" s="23"/>
+      <c r="D7" s="24">
+        <v>12</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="32.05" customHeight="1">
+      <c r="A8" s="25">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s" s="26">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" ht="32.05" customHeight="1">
-      <c r="A8" s="23">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s" s="24">
+      <c r="C8" s="27"/>
+      <c r="D8" s="28">
         <v>10</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26">
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="20.1" customHeight="1">
+      <c r="A9" s="29">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s" s="30">
+        <v>11</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="32.05" customHeight="1">
+      <c r="A10" s="17">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" ht="32.05" customHeight="1">
+      <c r="A11" s="17">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s" s="18">
+        <v>13</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="17">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" ht="20.1" customHeight="1">
-      <c r="A9" s="27">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s" s="28">
+      <c r="B12" t="s" s="18">
+        <v>14</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20">
+        <v>25</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" ht="32.1" customHeight="1">
+      <c r="A13" s="33">
         <v>11</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30">
+      <c r="B13" t="s" s="34">
+        <v>15</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36">
+        <v>15</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" ht="32.1" customHeight="1">
+      <c r="A14" s="29">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s" s="30">
+        <v>16</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32">
+        <v>15</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="17">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s" s="18">
+        <v>17</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20">
+        <v>5</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" ht="32.05" customHeight="1">
+      <c r="A16" s="17">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s" s="18">
+        <v>18</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20">
+        <v>5</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" ht="32.05" customHeight="1">
+      <c r="A17" s="17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s" s="18">
+        <v>19</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20">
+        <v>10</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" ht="20.1" customHeight="1">
+      <c r="A18" s="33">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s" s="34">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" ht="32.05" customHeight="1">
-      <c r="A10" s="15">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s" s="16">
-        <v>12</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" ht="32.05" customHeight="1">
-      <c r="A11" s="15">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s" s="16">
-        <v>13</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18">
+      <c r="C18" s="35"/>
+      <c r="D18" s="36">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="15">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s" s="16">
-        <v>14</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" ht="32.1" customHeight="1">
-      <c r="A13" s="31">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s" s="32">
-        <v>15</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" ht="32.1" customHeight="1">
-      <c r="A14" s="27">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s" s="28">
-        <v>16</v>
-      </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s" s="16">
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" ht="32.1" customHeight="1">
+      <c r="A19" s="29">
         <v>17</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18">
+      <c r="B19" t="s" s="30">
+        <v>21</v>
+      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" ht="32.05" customHeight="1">
-      <c r="A16" s="15">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s" s="16">
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" s="17">
         <v>18</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18">
+      <c r="B20" t="s" s="18">
+        <v>22</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" ht="32.05" customHeight="1">
-      <c r="A17" s="15">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s" s="16">
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" ht="56.05" customHeight="1">
+      <c r="A21" s="17">
         <v>19</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" ht="20.1" customHeight="1">
-      <c r="A18" s="31">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s" s="32">
+      <c r="B21" t="s" s="18">
+        <v>23</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20">
+        <v>5</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" s="17">
         <v>20</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34">
+      <c r="B22" t="s" s="18">
+        <v>24</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" ht="32.1" customHeight="1">
-      <c r="A19" s="27">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s" s="28">
-        <v>21</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="15">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s" s="16">
-        <v>22</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" ht="56.05" customHeight="1">
-      <c r="A21" s="15">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="15">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s" s="16">
-        <v>24</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18">
-        <v>5</v>
-      </c>
+      <c r="E22" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
update product backlog according to sprint backlogs
</commit_message>
<xml_diff>
--- a/process/ProductBacklog.xlsx
+++ b/process/ProductBacklog.xlsx
@@ -5,13 +5,13 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Product backlog" sheetId="1" r:id="rId4"/>
+    <sheet name="Foglio 1 - Product backlog" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Product backlog</t>
   </si>
@@ -55,6 +55,9 @@
     <t>Realizzazione di un plausibile algoritmo di propagazione del virus all’interno di ciascun posto (contando mascherine e una singola distanza soglia)</t>
   </si>
   <si>
+    <t>Implementazione di funzioni di movimento, per gestire gli spostamenti delle persone all'interno degli spazi di movimento</t>
+  </si>
+  <si>
     <t>Creazione automatica del dominio (città, posti e persone, con i relativi piani)</t>
   </si>
   <si>
@@ -64,28 +67,19 @@
     <t>Introduzione di attori per incapsulare il comportamento di ciascuna persona e simularne la vita</t>
   </si>
   <si>
-    <t>Funzionalità per reperire i posti di un certo tipo in una data città/provincia</t>
-  </si>
-  <si>
-    <t>Introduzione del quadro clinico, per gestire la fragilità di una persona al virus sulla base delle patologie pregresse (e quindi la possibilità di morte)</t>
+    <t>Implementazione dei diversi tipi di grafici e creazione di mappe raffiguranti il numero casi</t>
   </si>
   <si>
     <t>Raffinamento della GUI, con la possibilità di specificare i principali parametri in input, navigare tra i diversi grafici visualizzando le informazioni desiderate</t>
   </si>
   <si>
-    <t>Introduzione del concetto di tamponi</t>
-  </si>
-  <si>
     <t>Fornire la possibilità di effettuare più run (simulazioni) e visualizzare i risultati desiderati con la loro media</t>
   </si>
   <si>
-    <t>Considerare la possibilità di visite a parenti fuori regione</t>
-  </si>
-  <si>
-    <t>Raffinare il calcolo del rischio del contagio considerando tempi di incubazione e distanza tra persone (es. funzione che data una distanza calcola un fattore di aggiustamento della probabilità di contagio ottenuta in precedenza considerando solo le mascherine)</t>
-  </si>
-  <si>
-    <t>Introduzione del concetto di vacanze e hotel</t>
+    <t>Completamento della creazione dei posti del dominio</t>
+  </si>
+  <si>
+    <t>Raffinare il calcolo del rischio del contagio considerando distanza tra persone (es. funzione che data una distanza calcola un fattore di aggiustamento della probabilità di contagio ottenuta in precedenza considerando solo le mascherine)</t>
   </si>
 </sst>
 </file>
@@ -95,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -107,18 +101,13 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,14 +126,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="29">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -156,55 +139,20 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -224,335 +172,371 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
         <color indexed="13"/>
-      </right>
-      <top style="thin">
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
         <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
         <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
         <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
         <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
         <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
         <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
         <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
         <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,119 +546,131 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -694,10 +690,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffbfbfbf"/>
@@ -718,10 +712,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="A7A7A7"/>
+        <a:srgbClr val="5E5E5E"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="535353"/>
+        <a:srgbClr val="D5D5D5"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -898,14 +892,11 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
+          <a:srgbClr val="000000"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -914,34 +905,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica Neue Medium"/>
+            <a:ea typeface="Helvetica Neue Medium"/>
+            <a:cs typeface="Helvetica Neue Medium"/>
+            <a:sym typeface="Helvetica Neue Medium"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1189,12 +1180,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1485,7 +1476,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1763,301 +1754,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="61.3516" style="1" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.3438" style="1" customWidth="1"/>
+    <col min="3" max="4" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" ht="32.25" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
     </row>
     <row r="3" ht="32.2" customHeight="1">
-      <c r="A3" s="9">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="10">
+      <c r="B3" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12">
+      <c r="C3" s="7"/>
+      <c r="D3" s="8">
         <v>5</v>
       </c>
-      <c r="E3" s="8"/>
     </row>
     <row r="4" ht="32" customHeight="1">
-      <c r="A4" s="13">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="14">
+      <c r="B4" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16">
+      <c r="C4" s="11"/>
+      <c r="D4" s="12">
         <v>6</v>
       </c>
-      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" s="17">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" t="s" s="18">
+      <c r="B5" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20">
+      <c r="C5" s="15"/>
+      <c r="D5" s="16">
         <v>12</v>
       </c>
-      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" t="s" s="18">
+      <c r="B6" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
-      <c r="A7" s="21">
+      <c r="A7" s="17">
         <v>5</v>
       </c>
-      <c r="B7" t="s" s="22">
+      <c r="B7" t="s" s="18">
         <v>9</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24">
+      <c r="C7" s="19"/>
+      <c r="D7" s="20">
         <v>12</v>
       </c>
-      <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="32.05" customHeight="1">
-      <c r="A8" s="25">
+    <row r="8" ht="32.2" customHeight="1">
+      <c r="A8" s="21">
         <v>6</v>
       </c>
-      <c r="B8" t="s" s="26">
+      <c r="B8" t="s" s="22">
         <v>10</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24">
         <v>10</v>
       </c>
-      <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="20.1" customHeight="1">
-      <c r="A9" s="29">
+    <row r="9" ht="20.25" customHeight="1">
+      <c r="A9" s="25">
         <v>7</v>
       </c>
-      <c r="B9" t="s" s="30">
+      <c r="B9" t="s" s="26">
         <v>11</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32">
+      <c r="C9" s="27"/>
+      <c r="D9" s="28">
         <v>20</v>
       </c>
-      <c r="E9" s="8"/>
     </row>
     <row r="10" ht="32.05" customHeight="1">
-      <c r="A10" s="17">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" t="s" s="18">
+      <c r="B10" t="s" s="14">
         <v>12</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20">
+      <c r="C10" s="15"/>
+      <c r="D10" s="16">
         <v>3</v>
       </c>
-      <c r="E10" s="8"/>
     </row>
     <row r="11" ht="32.05" customHeight="1">
-      <c r="A11" s="17">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B11" t="s" s="18">
+      <c r="B11" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20">
+      <c r="C11" s="15"/>
+      <c r="D11" s="16">
         <v>5</v>
       </c>
-      <c r="E11" s="8"/>
     </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="17">
+    <row r="12" ht="32.05" customHeight="1">
+      <c r="A12" s="29"/>
+      <c r="B12" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="13">
         <v>10</v>
       </c>
-      <c r="B12" t="s" s="18">
-        <v>14</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20">
+      <c r="B13" t="s" s="14">
+        <v>15</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16">
         <v>25</v>
       </c>
-      <c r="E12" s="8"/>
     </row>
-    <row r="13" ht="32.1" customHeight="1">
-      <c r="A13" s="33">
+    <row r="14" ht="32.25" customHeight="1">
+      <c r="A14" s="30">
         <v>11</v>
       </c>
-      <c r="B13" t="s" s="34">
+      <c r="B14" t="s" s="31">
+        <v>16</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33">
         <v>15</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36">
+    </row>
+    <row r="15" ht="32.25" customHeight="1">
+      <c r="A15" s="25">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28">
         <v>15</v>
       </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" ht="32.1" customHeight="1">
-      <c r="A14" s="29">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s" s="30">
-        <v>16</v>
-      </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32">
-        <v>15</v>
-      </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="17">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s" s="18">
-        <v>17</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20">
-        <v>5</v>
-      </c>
-      <c r="E15" s="8"/>
     </row>
     <row r="16" ht="32.05" customHeight="1">
-      <c r="A16" s="17">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s" s="18">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s" s="14">
         <v>18</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20">
-        <v>5</v>
-      </c>
-      <c r="E16" s="8"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" ht="32.05" customHeight="1">
-      <c r="A17" s="17">
+      <c r="A17" s="13">
         <v>15</v>
       </c>
-      <c r="B17" t="s" s="18">
+      <c r="B17" t="s" s="14">
         <v>19</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20">
+      <c r="C17" s="15"/>
+      <c r="D17" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" ht="32.05" customHeight="1">
+      <c r="A18" s="13">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" ht="20.1" customHeight="1">
+      <c r="A19" s="34">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s" s="35">
+        <v>21</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37">
         <v>10</v>
       </c>
-      <c r="E17" s="8"/>
     </row>
-    <row r="18" ht="20.1" customHeight="1">
-      <c r="A18" s="33">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s" s="34">
-        <v>20</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36">
+    <row r="20" ht="44.3" customHeight="1">
+      <c r="A20" s="38">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s" s="39">
+        <v>22</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41">
         <v>5</v>
       </c>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" ht="32.1" customHeight="1">
-      <c r="A19" s="29">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s" s="30">
-        <v>21</v>
-      </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32">
-        <v>5</v>
-      </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="17">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s" s="18">
-        <v>22</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20">
-        <v>5</v>
-      </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" ht="56.05" customHeight="1">
-      <c r="A21" s="17">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s" s="18">
-        <v>23</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20">
-        <v>5</v>
-      </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="17">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s" s="18">
-        <v>24</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20">
-        <v>5</v>
-      </c>
-      <c r="E22" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>